<commit_message>
small changes in methods loading datasets
</commit_message>
<xml_diff>
--- a/doc/categories-wp.xlsx
+++ b/doc/categories-wp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1360" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>contributing-to-amidst</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>other</t>
+  </si>
+  <si>
+    <t>Latent variable models</t>
+  </si>
+  <si>
+    <t>Wekalink</t>
   </si>
 </sst>
 </file>
@@ -495,7 +501,7 @@
   <dimension ref="A4:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -666,11 +672,31 @@
         <f t="shared" si="0"/>
         <v>0.6.0</v>
       </c>
+      <c r="F14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="2" t="str">
+        <f>CONCATENATE(G14,"-",SUBSTITUTE(A14,".",""))</f>
+        <v>latent-var-models-060</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>0.6.0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="2" t="str">
+        <f>CONCATENATE(G15,"-",SUBSTITUTE(A15,".",""))</f>
+        <v>wekalink-060</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Xdoclint error with mvn3
</commit_message>
<xml_diff>
--- a/doc/categories-wp.xlsx
+++ b/doc/categories-wp.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rcabanas/GoogleDrive/AAU/amidst_rcabanas/repo/toolbox/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rcabanas/GoogleDrive/UAL/amidst/repo/toolbox/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40900" yWindow="3080" windowWidth="11820" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,9 +62,6 @@
     <t>Slug</t>
   </si>
   <si>
-    <t>Contributing to AMIDST</t>
-  </si>
-  <si>
     <t>Slug with version</t>
   </si>
   <si>
@@ -74,12 +71,6 @@
     <t>basic-steps-contributing</t>
   </si>
   <si>
-    <t>Examples</t>
-  </si>
-  <si>
-    <t>First steps</t>
-  </si>
-  <si>
     <t>Getting Started</t>
   </si>
   <si>
@@ -122,9 +113,6 @@
     <t>javadoc</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>other</t>
   </si>
   <si>
@@ -149,9 +137,6 @@
     <t>Sparklink</t>
   </si>
   <si>
-    <t>General Information</t>
-  </si>
-  <si>
     <t>general-information</t>
   </si>
   <si>
@@ -161,10 +146,25 @@
     <t>about-amidst</t>
   </si>
   <si>
-    <t>0.7.1</t>
-  </si>
-  <si>
     <t>v0.7.1</t>
+  </si>
+  <si>
+    <t>0.7.2</t>
+  </si>
+  <si>
+    <t>A. General Information</t>
+  </si>
+  <si>
+    <t>B. Examples</t>
+  </si>
+  <si>
+    <t>C. First steps</t>
+  </si>
+  <si>
+    <t>D. Contributing to AMIDST</t>
+  </si>
+  <si>
+    <t>E. Other</t>
   </si>
 </sst>
 </file>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F9" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="F3" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,7 +549,7 @@
     <col min="8" max="8" width="25.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -563,7 +563,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -572,446 +572,497 @@
         <v>11</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B5" t="str">
         <f>SUBSTITUTE(A5,".","-")</f>
-        <v>0-7-1</v>
+        <v>0-7-2</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="2" t="str">
         <f>CONCATENATE(D5,"-",SUBSTITUTE(A5,".",""))</f>
-        <v>contributing-to-amidst-071</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>contributing-to-amidst-072</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="str">
         <f>A5</f>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
         <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
       </c>
       <c r="H6" s="2" t="str">
         <f>CONCATENATE(G6,"-",SUBSTITUTE(A6,".",""))</f>
-        <v>basic-steps-contributing-071</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>basic-steps-contributing-072</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="str">
         <f t="shared" ref="A7:A37" si="0">A6</f>
-        <v>0.7.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.7.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="I8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
       </c>
       <c r="E9" s="2" t="str">
         <f>CONCATENATE(D9,"-",SUBSTITUTE(A9,".",""))</f>
-        <v>examples-071</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>examples-072</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="F10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G10" t="s">
         <v>3</v>
       </c>
       <c r="H10" s="2" t="str">
-        <f t="shared" ref="H10:H15" si="1">CONCATENATE(G10,"-",SUBSTITUTE(A10,".",""))</f>
-        <v>dbnetworks-071</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <f>CONCATENATE(G10,"-",SUBSTITUTE(A10,".",""))</f>
+        <v>dbnetworks-072</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G11" t="s">
         <v>4</v>
       </c>
       <c r="H11" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>flinklink-071</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <f>CONCATENATE(G11,"-",SUBSTITUTE(A11,".",""))</f>
+        <v>flinklink-072</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G12" t="s">
         <v>2</v>
       </c>
       <c r="H12" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>bnetworks-071</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" ref="H10:H15" si="1">CONCATENATE(G12,"-",SUBSTITUTE(A12,".",""))</f>
+        <v>bnetworks-072</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H13" s="2" t="str">
         <f>CONCATENATE(G13,"-",SUBSTITUTE(A13,".",""))</f>
-        <v>sparklink-071</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>sparklink-072</v>
+      </c>
+      <c r="J13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H14" s="2" t="str">
         <f>CONCATENATE(G14,"-",SUBSTITUTE(A14,".",""))</f>
-        <v>latent-var-models-071</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>latent-var-models-072</v>
+      </c>
+      <c r="J14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>wekalink-071</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+        <v>wekalink-072</v>
+      </c>
+      <c r="J15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
       </c>
       <c r="E16" s="2" t="str">
         <f>CONCATENATE(D16,"-",SUBSTITUTE(A16,".",""))</f>
-        <v>first-steps-071</v>
+        <v>first-steps-072</v>
+      </c>
+      <c r="J16">
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="F17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G17" t="s">
         <v>6</v>
       </c>
       <c r="H17" s="2" t="str">
         <f>CONCATENATE(G17,"-",SUBSTITUTE(A17,".",""))</f>
-        <v>generating-packages-071</v>
+        <v>generating-packages-072</v>
+      </c>
+      <c r="J17">
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="F18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G18" t="s">
         <v>7</v>
       </c>
       <c r="H18" s="2" t="str">
         <f>CONCATENATE(G18,"-",SUBSTITUTE(A18,".",""))</f>
-        <v>getting-started-071</v>
+        <v>getting-started-072</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="F19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G19" t="s">
         <v>8</v>
       </c>
       <c r="H19" s="2" t="str">
         <f>CONCATENATE(G19,"-",SUBSTITUTE(A19,".",""))</f>
-        <v>installing-local-repository-071</v>
+        <v>installing-local-repository-072</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="F20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G20" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H20" s="2" t="str">
         <f>CONCATENATE(G20,"-",SUBSTITUTE(A20,".",""))</f>
-        <v>loading-dependences-071</v>
+        <v>loading-dependences-072</v>
+      </c>
+      <c r="J20">
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="F21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G21" t="s">
         <v>9</v>
       </c>
       <c r="H21" s="2" t="str">
         <f>CONCATENATE(G21,"-",SUBSTITUTE(A21,".",""))</f>
-        <v>requirements-071</v>
+        <v>requirements-072</v>
+      </c>
+      <c r="J21">
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E25" s="4" t="str">
         <f>CONCATENATE(D25,"-",SUBSTITUTE(A25,".",""))</f>
-        <v>tutorials-071</v>
+        <v>tutorials-072</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="4"/>
       <c r="I25" s="3"/>
       <c r="K25" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
       <c r="F26" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H26" s="4" t="str">
         <f>CONCATENATE(G26,"-",SUBSTITUTE(A26,".",""))</f>
-        <v>latent-var-models-071</v>
+        <v>latent-var-models-072</v>
       </c>
       <c r="I26" s="3"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
       <c r="F27" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H27" s="4" t="str">
         <f>CONCATENATE(G27,"-",SUBSTITUTE(A27,".",""))</f>
-        <v>wekalink-071</v>
+        <v>wekalink-072</v>
       </c>
       <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="D29" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E29" s="2" t="str">
         <f>CONCATENATE(D29,"-",SUBSTITUTE(A29,".",""))</f>
-        <v>other-071</v>
+        <v>other-072</v>
+      </c>
+      <c r="J29">
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="F30" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G30" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H30" s="2" t="str">
         <f>CONCATENATE(G30,"-",SUBSTITUTE(A30,".",""))</f>
-        <v>javadoc-071</v>
+        <v>javadoc-072</v>
+      </c>
+      <c r="J30">
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.7.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="C33" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D33" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E33" s="2" t="str">
         <f>CONCATENATE(D33,"-",SUBSTITUTE(A33,".",""))</f>
-        <v>general-information-071</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+        <v>general-information-072</v>
+      </c>
+      <c r="J33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
       <c r="F34" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G34" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H34" s="2" t="str">
         <f>CONCATENATE(G34,"-",SUBSTITUTE(A34,".",""))</f>
-        <v>about-amidst-071</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+        <v>about-amidst-072</v>
+      </c>
+      <c r="J34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.7.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.7.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.7.1</v>
+        <v>0.7.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>